<commit_message>
#4 map ALL MEDM widgets to PyDM
</commit_message>
<xml_diff>
--- a/src/adl2pydm/ref/MEDM object names.xlsx
+++ b/src/adl2pydm/ref/MEDM object names.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pete\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D06AFC3E-96CD-413C-A22C-FF750FEF0397}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971ECD3E-C395-4D29-848B-AF96EF3215EB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="0" windowWidth="20580" windowHeight="8430" xr2:uid="{B0D9D1BE-AD8A-4F3C-80AC-829F4AF04EDD}"/>
+    <workbookView xWindow="9945" yWindow="-14925" windowWidth="18270" windowHeight="11835" xr2:uid="{B0D9D1BE-AD8A-4F3C-80AC-829F4AF04EDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="123">
   <si>
     <t>description</t>
   </si>
@@ -324,21 +324,12 @@
     <t>PyDMEmbeddedDisplay</t>
   </si>
   <si>
-    <t>?PyDMEnumButton</t>
-  </si>
-  <si>
     <t>PyDMPushButton</t>
   </si>
   <si>
-    <t>?PyDMScaleIndicator</t>
-  </si>
-  <si>
     <t>MEDM symbol</t>
   </si>
   <si>
-    <t>PyDMLineEdit + readOnly=True</t>
-  </si>
-  <si>
     <t>python widgets</t>
   </si>
   <si>
@@ -375,13 +366,34 @@
     <t>editable text that goes to PV</t>
   </si>
   <si>
-    <t>text that is updated from PV</t>
-  </si>
-  <si>
     <t>static text</t>
   </si>
   <si>
     <t>needle gauge display</t>
+  </si>
+  <si>
+    <t>PyDMEnumButton</t>
+  </si>
+  <si>
+    <t>PyDMScaleIndicator</t>
+  </si>
+  <si>
+    <t>text that is updated from PV,  + readOnly=True</t>
+  </si>
+  <si>
+    <t>PyDMDrawingRectangle</t>
+  </si>
+  <si>
+    <t>PyDMSpinbox</t>
+  </si>
+  <si>
+    <t>not sure about this assignment</t>
+  </si>
+  <si>
+    <t>PyDMByteIndicator</t>
+  </si>
+  <si>
+    <t>PyDMEnumComboBox</t>
   </si>
 </sst>
 </file>
@@ -448,9 +460,15 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BAE874CD-7543-4415-8EF6-CF569CC564A9}" name="Table1" displayName="Table1" ref="B3:I58" totalsRowShown="0">
-  <autoFilter ref="B3:I58" xr:uid="{94757081-4D69-40B1-A5AA-8921CB453007}"/>
-  <sortState ref="B4:G58">
-    <sortCondition ref="B3:B58"/>
+  <autoFilter ref="B3:I58" xr:uid="{94757081-4D69-40B1-A5AA-8921CB453007}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="widget"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState ref="B4:I58">
+    <sortCondition ref="C3:C58"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{658C3648-9555-4284-A3E9-0865DAD282E9}" name="MEDM symbol"/>
@@ -769,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6474B7C3-C197-4CB8-9D29-AC36C37969BA}">
   <dimension ref="B3:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34:H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,7 +805,7 @@
   <sheetData>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
         <v>70</v>
@@ -805,13 +823,13 @@
         <v>78</v>
       </c>
       <c r="H3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -833,7 +851,7 @@
         <v>"&lt;&lt;basic attribute&gt;&gt;" : dict(type=""),</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -855,7 +873,7 @@
         <v>"&lt;&lt;color map&gt;&gt;" : dict(type=""),</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -877,78 +895,78 @@
         <v>"&lt;&lt;color rules&gt;&gt;" : dict(type=""),</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H7" s="1" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
+        <v>"attr" : dict(type="nested", pydm_widget="---"),</v>
+      </c>
+      <c r="I7" s="2" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
+        <v>"attr" : dict(type="nested"),</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" t="s">
         <v>71</v>
       </c>
-      <c r="E7" t="s">
-        <v>68</v>
-      </c>
-      <c r="G7" t="s">
-        <v>87</v>
-      </c>
-      <c r="H7" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"arc" : dict(type="static", pydm_widget="PyDMDrawingArc"),</v>
-      </c>
-      <c r="I7" s="3" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"arc" : dict(type="static"),</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" t="s">
-        <v>76</v>
-      </c>
       <c r="G8" s="1" t="s">
         <v>79</v>
       </c>
       <c r="H8" s="1" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"attr" : dict(type="nested", pydm_widget="---"),</v>
+        <v>"basic attribute" : dict(type="static", pydm_widget="---"),</v>
       </c>
       <c r="I8" s="2" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"attr" : dict(type="nested"),</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+        <v>"basic attribute" : dict(type="static"),</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
-      </c>
-      <c r="H9" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"bar" : dict(type="monitor", pydm_widget=""),</v>
-      </c>
-      <c r="I9" s="3" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"bar" : dict(type="monitor"),</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H9" s="1" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
+        <v>"children" : dict(type="", pydm_widget="---"),</v>
+      </c>
+      <c r="I9" s="2" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
+        <v>"children" : dict(type=""),</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
         <v>53</v>
@@ -956,299 +974,302 @@
       <c r="D10" t="s">
         <v>71</v>
       </c>
+      <c r="E10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" t="s">
+        <v>104</v>
+      </c>
       <c r="G10" s="1" t="s">
         <v>79</v>
       </c>
       <c r="H10" s="1" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"basic attribute" : dict(type="static", pydm_widget="---"),</v>
+        <v>"color map" : dict(type="static", pydm_widget="---"),</v>
       </c>
       <c r="I10" s="2" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"basic attribute" : dict(type="static"),</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+        <v>"color map" : dict(type="static"),</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
-        <v>68</v>
-      </c>
-      <c r="H11" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"byte" : dict(type="monitor", pydm_widget=""),</v>
-      </c>
-      <c r="I11" s="3" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"byte" : dict(type="monitor"),</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" s="1" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
+        <v>"colors" : dict(type="", pydm_widget="---"),</v>
+      </c>
+      <c r="I11" s="2" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
+        <v>"colors" : dict(type=""),</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="F12" t="s">
-        <v>84</v>
-      </c>
-      <c r="G12" t="s">
-        <v>97</v>
-      </c>
-      <c r="H12" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"cartesian plot" : dict(type="monitor", pydm_widget="PyDMScatterPlot"),</v>
-      </c>
-      <c r="I12" s="3" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"cartesian plot" : dict(type="monitor"),</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H12" s="1" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
+        <v>"control" : dict(type="nested", pydm_widget="---"),</v>
+      </c>
+      <c r="I12" s="2" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
+        <v>"control" : dict(type="nested"),</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
         <v>53</v>
       </c>
+      <c r="D13" t="s">
+        <v>71</v>
+      </c>
       <c r="E13" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
       <c r="F13" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H13" s="1" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"children" : dict(type="", pydm_widget="---"),</v>
-      </c>
-      <c r="I13" s="2" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"children" : dict(type=""),</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="G13" t="s">
+        <v>80</v>
+      </c>
+      <c r="H13" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
+        <v>"display" : dict(type="static", pydm_widget="QWidget"),</v>
+      </c>
+      <c r="I13" s="3" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
+        <v>"display" : dict(type="static"),</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E14" t="s">
-        <v>68</v>
-      </c>
-      <c r="G14" t="s">
-        <v>99</v>
-      </c>
-      <c r="H14" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"choice button" : dict(type="controller", pydm_widget="?PyDMEnumButton"),</v>
-      </c>
-      <c r="I14" s="3" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"choice button" : dict(type="controller"),</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H14" s="1" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
+        <v>"dl_color" : dict(type="nested", pydm_widget="---"),</v>
+      </c>
+      <c r="I14" s="2" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
+        <v>"dl_color" : dict(type="nested"),</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
         <v>53</v>
       </c>
-      <c r="D15" t="s">
+      <c r="F15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H15" s="1" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
+        <v>"dl_color_rule" : dict(type="", pydm_widget="---"),</v>
+      </c>
+      <c r="I15" s="2" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
+        <v>"dl_color_rule" : dict(type=""),</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" t="s">
         <v>71</v>
       </c>
-      <c r="E15" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="F16" t="s">
         <v>107</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H15" s="1" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"color map" : dict(type="static", pydm_widget="---"),</v>
-      </c>
-      <c r="I15" s="2" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"color map" : dict(type="static"),</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" t="s">
-        <v>55</v>
-      </c>
       <c r="G16" s="1" t="s">
         <v>79</v>
       </c>
       <c r="H16" s="1" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"colors" : dict(type="", pydm_widget="---"),</v>
+        <v>"dynamic attribute" : dict(type="static", pydm_widget="---"),</v>
       </c>
       <c r="I16" s="2" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"colors" : dict(type=""),</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+        <v>"dynamic attribute" : dict(type="static"),</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="C17" t="s">
-        <v>106</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>76</v>
+        <v>71</v>
+      </c>
+      <c r="E17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" t="s">
+        <v>81</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>79</v>
       </c>
       <c r="H17" s="1" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"command[0]" : dict(type="nested", pydm_widget="---"),</v>
+        <v>"falling line" : dict(type="static", pydm_widget="---"),</v>
       </c>
       <c r="I17" s="2" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"command[0]" : dict(type="nested"),</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+        <v>"falling line" : dict(type="static"),</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
         <v>71</v>
       </c>
       <c r="E18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F18" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18" t="s">
-        <v>86</v>
-      </c>
-      <c r="H18" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"composite" : dict(type="static", pydm_widget="PyDMFrame"),</v>
-      </c>
-      <c r="I18" s="3" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"composite" : dict(type="static"),</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H18" s="1" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
+        <v>"file" : dict(type="static", pydm_widget="---"),</v>
+      </c>
+      <c r="I18" s="2" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
+        <v>"file" : dict(type="static"),</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
         <v>53</v>
       </c>
-      <c r="D19" t="s">
-        <v>76</v>
-      </c>
-      <c r="F19" t="s">
-        <v>108</v>
-      </c>
       <c r="G19" s="1" t="s">
         <v>79</v>
       </c>
       <c r="H19" s="1" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"control" : dict(type="nested", pydm_widget="---"),</v>
+        <v>"limits" : dict(type="", pydm_widget="---"),</v>
       </c>
       <c r="I19" s="2" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"control" : dict(type="nested"),</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+        <v>"limits" : dict(type=""),</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
         <v>53</v>
       </c>
-      <c r="D20" t="s">
-        <v>71</v>
-      </c>
-      <c r="E20" t="s">
-        <v>67</v>
-      </c>
       <c r="F20" t="s">
-        <v>109</v>
-      </c>
-      <c r="G20" t="s">
-        <v>80</v>
-      </c>
-      <c r="H20" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"display" : dict(type="static", pydm_widget="QWidget"),</v>
-      </c>
-      <c r="I20" s="3" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"display" : dict(type="static"),</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H20" s="1" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
+        <v>"mod" : dict(type="", pydm_widget="---"),</v>
+      </c>
+      <c r="I20" s="2" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
+        <v>"mod" : dict(type=""),</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>106</v>
+        <v>53</v>
       </c>
       <c r="D21" t="s">
         <v>76</v>
       </c>
+      <c r="F21" t="s">
+        <v>109</v>
+      </c>
       <c r="G21" s="1" t="s">
         <v>79</v>
       </c>
       <c r="H21" s="1" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"display[0]" : dict(type="nested", pydm_widget="---"),</v>
+        <v>"monitor" : dict(type="nested", pydm_widget="---"),</v>
       </c>
       <c r="I21" s="2" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"display[0]" : dict(type="nested"),</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+        <v>"monitor" : dict(type="nested"),</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
         <v>53</v>
@@ -1257,54 +1278,51 @@
         <v>76</v>
       </c>
       <c r="E22" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="F22" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>79</v>
       </c>
       <c r="H22" s="1" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"dl_color" : dict(type="nested", pydm_widget="---"),</v>
+        <v>"object" : dict(type="nested", pydm_widget="---"),</v>
       </c>
       <c r="I22" s="2" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"dl_color" : dict(type="nested"),</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+        <v>"object" : dict(type="nested"),</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
         <v>53</v>
       </c>
-      <c r="F23" t="s">
-        <v>64</v>
+      <c r="D23" t="s">
+        <v>76</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>79</v>
       </c>
       <c r="H23" s="1" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"dl_color_rule" : dict(type="", pydm_widget="---"),</v>
+        <v>"plotcom" : dict(type="nested", pydm_widget="---"),</v>
       </c>
       <c r="I23" s="2" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"dl_color_rule" : dict(type=""),</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+        <v>"plotcom" : dict(type="nested"),</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
         <v>53</v>
-      </c>
-      <c r="D24" t="s">
-        <v>71</v>
       </c>
       <c r="F24" t="s">
         <v>110</v>
@@ -1314,150 +1332,126 @@
       </c>
       <c r="H24" s="1" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"dynamic attribute" : dict(type="static", pydm_widget="---"),</v>
+        <v>"points" : dict(type="", pydm_widget="---"),</v>
       </c>
       <c r="I24" s="2" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"dynamic attribute" : dict(type="static"),</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+        <v>"points" : dict(type=""),</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D25" t="s">
         <v>71</v>
       </c>
       <c r="E25" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="F25" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="H25" s="1" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"embedded display" : dict(type="static", pydm_widget="PyDMEmbeddedDisplay"),</v>
+        <v>"rising line" : dict(type="static", pydm_widget="---"),</v>
       </c>
       <c r="I25" s="2" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"embedded display" : dict(type="static"),</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+        <v>"rising line" : dict(type="static"),</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="C26" t="s">
         <v>53</v>
       </c>
-      <c r="D26" t="s">
-        <v>71</v>
-      </c>
-      <c r="E26" t="s">
-        <v>74</v>
-      </c>
-      <c r="F26" t="s">
-        <v>81</v>
-      </c>
       <c r="G26" s="1" t="s">
         <v>79</v>
       </c>
       <c r="H26" s="1" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"falling line" : dict(type="static", pydm_widget="---"),</v>
+        <v>"x_axis" : dict(type="", pydm_widget="---"),</v>
       </c>
       <c r="I26" s="2" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"falling line" : dict(type="static"),</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+        <v>"x_axis" : dict(type=""),</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="C27" t="s">
         <v>53</v>
       </c>
-      <c r="D27" t="s">
-        <v>71</v>
-      </c>
-      <c r="E27" t="s">
-        <v>67</v>
-      </c>
-      <c r="F27" t="s">
-        <v>111</v>
-      </c>
       <c r="G27" s="1" t="s">
         <v>79</v>
       </c>
       <c r="H27" s="1" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"file" : dict(type="static", pydm_widget="---"),</v>
+        <v>"y1_axis" : dict(type="", pydm_widget="---"),</v>
       </c>
       <c r="I27" s="2" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"file" : dict(type="static"),</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+        <v>"y1_axis" : dict(type=""),</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C28" t="s">
-        <v>52</v>
-      </c>
-      <c r="D28" t="s">
-        <v>31</v>
-      </c>
-      <c r="E28" t="s">
-        <v>68</v>
-      </c>
-      <c r="G28" t="s">
-        <v>90</v>
-      </c>
-      <c r="H28" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"image" : dict(type="monitor", pydm_widget="PyDMImageView"),</v>
-      </c>
-      <c r="I28" s="3" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"image" : dict(type="monitor"),</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H28" s="1" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
+        <v>"y2_axis" : dict(type="", pydm_widget="---"),</v>
+      </c>
+      <c r="I28" s="2" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
+        <v>"y2_axis" : dict(type=""),</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C29" t="s">
-        <v>52</v>
+        <v>103</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
-      </c>
-      <c r="E29" t="s">
-        <v>68</v>
-      </c>
-      <c r="H29" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"indicator" : dict(type="monitor", pydm_widget=""),</v>
-      </c>
-      <c r="I29" s="3" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"indicator" : dict(type="monitor"),</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H29" s="1" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
+        <v>"command[0]" : dict(type="nested", pydm_widget="---"),</v>
+      </c>
+      <c r="I29" s="2" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
+        <v>"command[0]" : dict(type="nested"),</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C30" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D30" t="s">
         <v>76</v>
@@ -1467,216 +1461,210 @@
       </c>
       <c r="H30" s="1" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
+        <v>"display[0]" : dict(type="nested", pydm_widget="---"),</v>
+      </c>
+      <c r="I30" s="2" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
+        <v>"display[0]" : dict(type="nested"),</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" t="s">
+        <v>76</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H31" s="1" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
         <v>"info[0]" : dict(type="nested", pydm_widget="---"),</v>
       </c>
-      <c r="I30" s="2" t="str">
+      <c r="I31" s="2" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
         <v>"info[0]" : dict(type="nested"),</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" t="s">
-        <v>53</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H31" s="1" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"limits" : dict(type="", pydm_widget="---"),</v>
-      </c>
-      <c r="I31" s="2" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"limits" : dict(type=""),</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>52</v>
+        <v>103</v>
       </c>
       <c r="D32" t="s">
-        <v>75</v>
-      </c>
-      <c r="E32" t="s">
-        <v>68</v>
-      </c>
-      <c r="F32" t="s">
-        <v>60</v>
-      </c>
-      <c r="G32" t="s">
-        <v>99</v>
-      </c>
-      <c r="H32" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"menu" : dict(type="controller", pydm_widget="?PyDMEnumButton"),</v>
-      </c>
-      <c r="I32" s="3" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"menu" : dict(type="controller"),</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H32" s="1" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
+        <v>"pen[0]" : dict(type="nested", pydm_widget="---"),</v>
+      </c>
+      <c r="I32" s="2" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
+        <v>"pen[0]" : dict(type="nested"),</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C33" t="s">
-        <v>52</v>
+        <v>103</v>
       </c>
       <c r="D33" t="s">
-        <v>75</v>
-      </c>
-      <c r="E33" t="s">
-        <v>68</v>
-      </c>
-      <c r="G33" t="s">
-        <v>100</v>
-      </c>
-      <c r="H33" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"message button" : dict(type="controller", pydm_widget="PyDMPushButton"),</v>
-      </c>
-      <c r="I33" s="3" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"message button" : dict(type="controller"),</v>
+        <v>76</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H33" s="1" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
+        <v>"trace[0]" : dict(type="nested", pydm_widget="---"),</v>
+      </c>
+      <c r="I33" s="2" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
+        <v>"trace[0]" : dict(type="nested"),</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="C34" t="s">
         <v>52</v>
       </c>
       <c r="D34" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="E34" t="s">
         <v>68</v>
       </c>
-      <c r="F34" t="s">
-        <v>118</v>
-      </c>
       <c r="G34" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="H34" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"meter" : dict(type="monitor", pydm_widget="?PyDMScaleIndicator"),</v>
+        <v>"arc" : dict(type="static", pydm_widget="PyDMDrawingArc"),</v>
       </c>
       <c r="I34" s="3" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"meter" : dict(type="monitor"),</v>
+        <v>"arc" : dict(type="static"),</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>53</v>
-      </c>
-      <c r="F35" t="s">
-        <v>58</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H35" s="1" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"mod" : dict(type="", pydm_widget="---"),</v>
-      </c>
-      <c r="I35" s="2" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"mod" : dict(type=""),</v>
+        <v>52</v>
+      </c>
+      <c r="D35" t="s">
+        <v>31</v>
+      </c>
+      <c r="E35" t="s">
+        <v>68</v>
+      </c>
+      <c r="G35" t="s">
+        <v>118</v>
+      </c>
+      <c r="H35" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
+        <v>"bar" : dict(type="monitor", pydm_widget="PyDMDrawingRectangle"),</v>
+      </c>
+      <c r="I35" s="3" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
+        <v>"bar" : dict(type="monitor"),</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" t="s">
         <v>31</v>
       </c>
-      <c r="C36" t="s">
-        <v>53</v>
-      </c>
-      <c r="D36" t="s">
-        <v>76</v>
-      </c>
-      <c r="F36" t="s">
-        <v>112</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H36" s="1" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"monitor" : dict(type="nested", pydm_widget="---"),</v>
-      </c>
-      <c r="I36" s="2" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"monitor" : dict(type="nested"),</v>
+      <c r="E36" t="s">
+        <v>68</v>
+      </c>
+      <c r="G36" t="s">
+        <v>121</v>
+      </c>
+      <c r="H36" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
+        <v>"byte" : dict(type="monitor", pydm_widget="PyDMByteIndicator"),</v>
+      </c>
+      <c r="I36" s="3" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
+        <v>"byte" : dict(type="monitor"),</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D37" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="E37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F37" t="s">
-        <v>57</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H37" s="1" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"object" : dict(type="nested", pydm_widget="---"),</v>
-      </c>
-      <c r="I37" s="2" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"object" : dict(type="nested"),</v>
+        <v>84</v>
+      </c>
+      <c r="G37" t="s">
+        <v>97</v>
+      </c>
+      <c r="H37" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
+        <v>"cartesian plot" : dict(type="monitor", pydm_widget="PyDMScatterPlot"),</v>
+      </c>
+      <c r="I37" s="3" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
+        <v>"cartesian plot" : dict(type="monitor"),</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="C38" t="s">
         <v>52</v>
       </c>
       <c r="D38" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E38" t="s">
         <v>68</v>
       </c>
       <c r="G38" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="H38" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"oval" : dict(type="static", pydm_widget="PyDMDrawingEllipse"),</v>
+        <v>"choice button" : dict(type="controller", pydm_widget="PyDMEnumComboBox"),</v>
       </c>
       <c r="I38" s="3" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"oval" : dict(type="static"),</v>
+        <v>"choice button" : dict(type="controller"),</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="C39" t="s">
         <v>52</v>
@@ -1688,155 +1676,185 @@
         <v>68</v>
       </c>
       <c r="F39" t="s">
-        <v>59</v>
+        <v>56</v>
+      </c>
+      <c r="G39" t="s">
+        <v>86</v>
       </c>
       <c r="H39" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"param" : dict(type="static", pydm_widget=""),</v>
+        <v>"composite" : dict(type="static", pydm_widget="PyDMFrame"),</v>
       </c>
       <c r="I39" s="3" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"param" : dict(type="static"),</v>
+        <v>"composite" : dict(type="static"),</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>35</v>
+        <v>91</v>
       </c>
       <c r="C40" t="s">
-        <v>106</v>
+        <v>52</v>
       </c>
       <c r="D40" t="s">
-        <v>76</v>
+        <v>71</v>
+      </c>
+      <c r="E40" t="s">
+        <v>68</v>
+      </c>
+      <c r="F40" t="s">
+        <v>92</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="H40" s="1" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"pen[0]" : dict(type="nested", pydm_widget="---"),</v>
+        <v>"embedded display" : dict(type="static", pydm_widget="PyDMEmbeddedDisplay"),</v>
       </c>
       <c r="I40" s="2" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"pen[0]" : dict(type="nested"),</v>
+        <v>"embedded display" : dict(type="static"),</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D41" t="s">
-        <v>76</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H41" s="1" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"plotcom" : dict(type="nested", pydm_widget="---"),</v>
-      </c>
-      <c r="I41" s="2" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"plotcom" : dict(type="nested"),</v>
+        <v>31</v>
+      </c>
+      <c r="E41" t="s">
+        <v>68</v>
+      </c>
+      <c r="G41" t="s">
+        <v>90</v>
+      </c>
+      <c r="H41" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
+        <v>"image" : dict(type="monitor", pydm_widget="PyDMImageView"),</v>
+      </c>
+      <c r="I41" s="3" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
+        <v>"image" : dict(type="monitor"),</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C42" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="D42" t="s">
+        <v>31</v>
+      </c>
+      <c r="E42" t="s">
+        <v>68</v>
       </c>
       <c r="F42" t="s">
-        <v>113</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H42" s="1" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"points" : dict(type="", pydm_widget="---"),</v>
-      </c>
-      <c r="I42" s="2" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"points" : dict(type=""),</v>
+        <v>120</v>
+      </c>
+      <c r="G42" t="s">
+        <v>94</v>
+      </c>
+      <c r="H42" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
+        <v>"indicator" : dict(type="monitor", pydm_widget="PyDMLineEdit"),</v>
+      </c>
+      <c r="I42" s="3" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
+        <v>"indicator" : dict(type="monitor"),</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C43" t="s">
         <v>52</v>
       </c>
       <c r="D43" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E43" t="s">
         <v>68</v>
       </c>
+      <c r="F43" t="s">
+        <v>60</v>
+      </c>
       <c r="G43" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="H43" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"polygon" : dict(type="static", pydm_widget="PyDMDrawingPolygon"),</v>
+        <v>"menu" : dict(type="controller", pydm_widget="PyDMEnumButton"),</v>
       </c>
       <c r="I43" s="3" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"polygon" : dict(type="static"),</v>
+        <v>"menu" : dict(type="controller"),</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C44" t="s">
         <v>52</v>
       </c>
       <c r="D44" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E44" t="s">
         <v>68</v>
       </c>
+      <c r="G44" t="s">
+        <v>99</v>
+      </c>
       <c r="H44" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"polyline" : dict(type="static", pydm_widget=""),</v>
+        <v>"message button" : dict(type="controller", pydm_widget="PyDMPushButton"),</v>
       </c>
       <c r="I44" s="3" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"polyline" : dict(type="static"),</v>
+        <v>"message button" : dict(type="controller"),</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C45" t="s">
         <v>52</v>
       </c>
       <c r="D45" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="E45" t="s">
         <v>68</v>
       </c>
+      <c r="F45" t="s">
+        <v>114</v>
+      </c>
+      <c r="G45" t="s">
+        <v>116</v>
+      </c>
       <c r="H45" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"rectangle" : dict(type="static", pydm_widget=""),</v>
+        <v>"meter" : dict(type="monitor", pydm_widget="PyDMScaleIndicator"),</v>
       </c>
       <c r="I45" s="3" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"rectangle" : dict(type="static"),</v>
+        <v>"meter" : dict(type="monitor"),</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C46" t="s">
         <v>52</v>
@@ -1847,24 +1865,21 @@
       <c r="E46" t="s">
         <v>68</v>
       </c>
-      <c r="F46" t="s">
-        <v>114</v>
-      </c>
       <c r="G46" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="H46" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"related display" : dict(type="static", pydm_widget="PyDMRelatedDisplayButton"),</v>
+        <v>"oval" : dict(type="static", pydm_widget="PyDMDrawingEllipse"),</v>
       </c>
       <c r="I46" s="3" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"related display" : dict(type="static"),</v>
-      </c>
-    </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+        <v>"oval" : dict(type="static"),</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="C47" t="s">
         <v>53</v>
@@ -1873,26 +1888,23 @@
         <v>71</v>
       </c>
       <c r="E47" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F47" t="s">
-        <v>81</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H47" s="1" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"rising line" : dict(type="static", pydm_widget="---"),</v>
-      </c>
-      <c r="I47" s="2" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"rising line" : dict(type="static"),</v>
+        <v>59</v>
+      </c>
+      <c r="H47" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
+        <v>"param" : dict(type="static", pydm_widget=""),</v>
+      </c>
+      <c r="I47" s="3" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
+        <v>"param" : dict(type="static"),</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C48" t="s">
         <v>52</v>
@@ -1903,52 +1915,46 @@
       <c r="E48" t="s">
         <v>68</v>
       </c>
-      <c r="F48" t="s">
-        <v>77</v>
-      </c>
       <c r="G48" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="H48" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"shell command" : dict(type="static", pydm_widget="PyDMShellCommand"),</v>
+        <v>"polygon" : dict(type="static", pydm_widget="PyDMDrawingPolygon"),</v>
       </c>
       <c r="I48" s="3" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"shell command" : dict(type="static"),</v>
+        <v>"polygon" : dict(type="static"),</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C49" t="s">
         <v>52</v>
       </c>
       <c r="D49" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="E49" t="s">
         <v>68</v>
       </c>
-      <c r="F49" t="s">
-        <v>83</v>
-      </c>
       <c r="G49" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H49" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"strip chart" : dict(type="monitor", pydm_widget="PyDMTimePlot"),</v>
+        <v>"polyline" : dict(type="static", pydm_widget="PyDMDrawingPolygon"),</v>
       </c>
       <c r="I49" s="3" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"strip chart" : dict(type="monitor"),</v>
+        <v>"polyline" : dict(type="static"),</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C50" t="s">
         <v>52</v>
@@ -1959,124 +1965,133 @@
       <c r="E50" t="s">
         <v>68</v>
       </c>
-      <c r="F50" t="s">
-        <v>117</v>
-      </c>
       <c r="G50" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="H50" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"text" : dict(type="static", pydm_widget="PyDMLabel"),</v>
+        <v>"rectangle" : dict(type="static", pydm_widget="PyDMDrawingRectangle"),</v>
       </c>
       <c r="I50" s="3" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"text" : dict(type="static"),</v>
+        <v>"rectangle" : dict(type="static"),</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C51" t="s">
         <v>52</v>
       </c>
       <c r="D51" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E51" t="s">
         <v>68</v>
       </c>
       <c r="F51" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G51" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H51" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"text entry" : dict(type="controller", pydm_widget="PyDMLineEdit"),</v>
+        <v>"related display" : dict(type="static", pydm_widget="PyDMRelatedDisplayButton"),</v>
       </c>
       <c r="I51" s="3" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"text entry" : dict(type="controller"),</v>
+        <v>"related display" : dict(type="static"),</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C52" t="s">
         <v>52</v>
       </c>
       <c r="D52" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="E52" t="s">
         <v>68</v>
       </c>
       <c r="F52" t="s">
-        <v>116</v>
+        <v>77</v>
       </c>
       <c r="G52" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="H52" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"text update" : dict(type="monitor", pydm_widget="PyDMLineEdit + readOnly=True"),</v>
+        <v>"shell command" : dict(type="static", pydm_widget="PyDMShellCommand"),</v>
       </c>
       <c r="I52" s="3" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"text update" : dict(type="monitor"),</v>
+        <v>"shell command" : dict(type="static"),</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C53" t="s">
-        <v>106</v>
+        <v>52</v>
       </c>
       <c r="D53" t="s">
-        <v>76</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H53" s="1" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"trace[0]" : dict(type="nested", pydm_widget="---"),</v>
-      </c>
-      <c r="I53" s="2" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"trace[0]" : dict(type="nested"),</v>
+        <v>31</v>
+      </c>
+      <c r="E53" t="s">
+        <v>68</v>
+      </c>
+      <c r="F53" t="s">
+        <v>83</v>
+      </c>
+      <c r="G53" t="s">
+        <v>85</v>
+      </c>
+      <c r="H53" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
+        <v>"strip chart" : dict(type="monitor", pydm_widget="PyDMTimePlot"),</v>
+      </c>
+      <c r="I53" s="3" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
+        <v>"strip chart" : dict(type="monitor"),</v>
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C54" t="s">
         <v>52</v>
       </c>
       <c r="D54" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E54" t="s">
         <v>68</v>
       </c>
+      <c r="F54" t="s">
+        <v>113</v>
+      </c>
+      <c r="G54" t="s">
+        <v>93</v>
+      </c>
       <c r="H54" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"valuator" : dict(type="controller", pydm_widget=""),</v>
+        <v>"text" : dict(type="static", pydm_widget="PyDMLabel"),</v>
       </c>
       <c r="I54" s="3" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"valuator" : dict(type="controller"),</v>
+        <v>"text" : dict(type="static"),</v>
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="C55" t="s">
         <v>52</v>
@@ -2087,70 +2102,103 @@
       <c r="E55" t="s">
         <v>68</v>
       </c>
+      <c r="F55" t="s">
+        <v>112</v>
+      </c>
+      <c r="G55" t="s">
+        <v>94</v>
+      </c>
       <c r="H55" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"wheel switch" : dict(type="controller", pydm_widget=""),</v>
+        <v>"text entry" : dict(type="controller", pydm_widget="PyDMLineEdit"),</v>
       </c>
       <c r="I55" s="3" t="str">
         <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"wheel switch" : dict(type="controller"),</v>
+        <v>"text entry" : dict(type="controller"),</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C56" t="s">
-        <v>53</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H56" s="1" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"x_axis" : dict(type="", pydm_widget="---"),</v>
-      </c>
-      <c r="I56" s="2" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"x_axis" : dict(type=""),</v>
+        <v>52</v>
+      </c>
+      <c r="D56" t="s">
+        <v>31</v>
+      </c>
+      <c r="E56" t="s">
+        <v>68</v>
+      </c>
+      <c r="F56" t="s">
+        <v>117</v>
+      </c>
+      <c r="G56" t="s">
+        <v>94</v>
+      </c>
+      <c r="H56" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
+        <v>"text update" : dict(type="monitor", pydm_widget="PyDMLineEdit"),</v>
+      </c>
+      <c r="I56" s="3" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
+        <v>"text update" : dict(type="monitor"),</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C57" t="s">
-        <v>53</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H57" s="1" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"y1_axis" : dict(type="", pydm_widget="---"),</v>
-      </c>
-      <c r="I57" s="2" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"y1_axis" : dict(type=""),</v>
+        <v>52</v>
+      </c>
+      <c r="D57" t="s">
+        <v>75</v>
+      </c>
+      <c r="E57" t="s">
+        <v>68</v>
+      </c>
+      <c r="F57" t="s">
+        <v>120</v>
+      </c>
+      <c r="G57" t="s">
+        <v>94</v>
+      </c>
+      <c r="H57" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
+        <v>"valuator" : dict(type="controller", pydm_widget="PyDMLineEdit"),</v>
+      </c>
+      <c r="I57" s="3" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
+        <v>"valuator" : dict(type="controller"),</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="C58" t="s">
-        <v>53</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H58" s="1" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
-        <v>"y2_axis" : dict(type="", pydm_widget="---"),</v>
-      </c>
-      <c r="I58" s="2" t="str">
-        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
-        <v>"y2_axis" : dict(type=""),</v>
+        <v>52</v>
+      </c>
+      <c r="D58" t="s">
+        <v>75</v>
+      </c>
+      <c r="E58" t="s">
+        <v>68</v>
+      </c>
+      <c r="F58" t="s">
+        <v>120</v>
+      </c>
+      <c r="G58" t="s">
+        <v>119</v>
+      </c>
+      <c r="H58" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;""", pydm_widget="""&amp;Table1[[#This Row],[PyDM widget]]&amp;"""),"</f>
+        <v>"wheel switch" : dict(type="controller", pydm_widget="PyDMSpinbox"),</v>
+      </c>
+      <c r="I58" s="3" t="str">
+        <f xml:space="preserve"> """"&amp;Table1[[#This Row],[MEDM symbol]]&amp;""" : dict(type="""&amp;Table1[[#This Row],[type]]&amp;"""),"</f>
+        <v>"wheel switch" : dict(type="controller"),</v>
       </c>
     </row>
   </sheetData>

</xml_diff>